<commit_message>
Add moneylender shops to forms
</commit_message>
<xml_diff>
--- a/OpenMapKit/hot_06_mfi.xlsx
+++ b/OpenMapKit/hot_06_mfi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>type</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>Vision Fund</t>
+  </si>
+  <si>
+    <t>Platinum Credit</t>
   </si>
   <si>
     <t>24/7</t>
@@ -364,7 +367,7 @@
   </sheetPr>
   <dimension ref="A1:Z65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -683,6 +686,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7040816326531"/>
     <col collapsed="false" hidden="false" max="6" min="4" style="0" width="11.5714285714286"/>
     <col collapsed="false" hidden="false" max="13" min="7" style="0" width="8.70918367346939"/>
@@ -740,10 +744,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1350,7 +1354,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>21</v>
       </c>
@@ -1384,10 +1388,16 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="9"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>42</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -1413,15 +1423,9 @@
       <c r="Z20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1450,10 +1454,10 @@
       <c r="A22" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D22" s="2"/>
@@ -1620,10 +1624,10 @@
       <c r="A27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="2"/>
@@ -1651,9 +1655,15 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="A28" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -1679,15 +1689,9 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>49</v>
-      </c>
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -1781,7 +1785,7 @@
       <c r="Z31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -1813,6 +1817,40 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1839,6 +1877,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
     <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.86224489795918"/>
     <col collapsed="false" hidden="false" max="12" min="7" style="0" width="8.70918367346939"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="17.2857142857143"/>
@@ -1846,10 +1885,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -1878,10 +1917,10 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>

</xml_diff>